<commit_message>
Added Schreibvorlage und Doku
Just the beginnig of something majestic
</commit_message>
<xml_diff>
--- a/Peter/Arbeitszeitabelle.xlsx
+++ b/Peter/Arbeitszeitabelle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr showObjects="none" filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4204148-F60F-4F69-ACEF-DEF7735BFE74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B19273-3F50-4854-B7DD-414B53026942}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Datum</t>
   </si>
@@ -181,6 +181,30 @@
   <si>
     <t>Besprechung mit Prof.Wurzinger programmierung</t>
   </si>
+  <si>
+    <t xml:space="preserve">Kleinstprogramme </t>
+  </si>
+  <si>
+    <t>Kleinstprogramme Wie mit Prof. Wurzinger ausgemacht(Programm Zeigt eine Kleine Wirkung</t>
+  </si>
+  <si>
+    <t>Kinecteinbindung</t>
+  </si>
+  <si>
+    <t>Probleme mit den OpenNi.java da nicht Vorhanden</t>
+  </si>
+  <si>
+    <t>Auslesen von Kinectdaten einbindung in das Rock Paper Scissors Programm</t>
+  </si>
+  <si>
+    <t>Besprechung mit Hr. Prof. Wurzinger &amp; Programmierung</t>
+  </si>
+  <si>
+    <t>Kinecteinbindung besprehung mit Hr. Wurzinger</t>
+  </si>
+  <si>
+    <t>Zählen der Bewegungen.</t>
+  </si>
 </sst>
 </file>
 
@@ -188,7 +212,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -281,7 +305,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -563,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,7 +1166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>43521</v>
       </c>
@@ -1153,10 +1177,82 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>43523</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>43525</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C51">
-        <f>SUM(C2:C49)</f>
-        <v>109</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>43526</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>43527</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>43528</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>43530</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>